<commit_message>
termino de mapa de gantt
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SEBASTIAN\Desktop\Proyecto_Algo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14319E9-C919-46D1-AFAE-24014F7BD663}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B035E1E5-8926-4548-915F-ADCC68CF4FC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="0" windowWidth="18675" windowHeight="15600" xr2:uid="{03B53AA5-B030-4197-B15D-A5F9E0DA3FFA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{03B53AA5-B030-4197-B15D-A5F9E0DA3FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
-  <si>
-    <t>Tarea</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Semana 12</t>
   </si>
@@ -69,13 +66,55 @@
   </si>
   <si>
     <t>Fin</t>
+  </si>
+  <si>
+    <t>sabado</t>
+  </si>
+  <si>
+    <t>domingo</t>
+  </si>
+  <si>
+    <t>Definición de las necesidades específicas</t>
+  </si>
+  <si>
+    <t>Inicio de la estructura del informe</t>
+  </si>
+  <si>
+    <t>Implementacion de clases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correcion de errores </t>
+  </si>
+  <si>
+    <t>Entrega Hito 2</t>
+  </si>
+  <si>
+    <t>Tareas</t>
+  </si>
+  <si>
+    <t>Diseño de interfaz de usuario</t>
+  </si>
+  <si>
+    <t>Diseño de tipos de datos</t>
+  </si>
+  <si>
+    <t>Selección de estructuras de datos</t>
+  </si>
+  <si>
+    <t>Implementacion de funcionalidades</t>
+  </si>
+  <si>
+    <t>correcion de errorres</t>
+  </si>
+  <si>
+    <t>Entrega de hito 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,8 +122,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,8 +149,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -164,18 +216,129 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -185,12 +348,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,139 +710,638 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F093C092-DA42-4723-9B3E-2E4A49CD9717}">
-  <dimension ref="A2:X5"/>
+  <dimension ref="A2:AE15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AB20" sqref="AB20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C2" s="3" t="s">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="3"/>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="7"/>
-      <c r="O2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="7"/>
-      <c r="T2" s="5" t="s">
+      <c r="K3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="7"/>
+      <c r="M3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB3" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE3" s="12" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="1" t="s">
+    <row r="4" spans="1:31" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="7">
+        <v>43766</v>
+      </c>
+      <c r="D4" s="9">
+        <v>43767</v>
+      </c>
+      <c r="E4" s="17"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="20"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="20"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="19"/>
+      <c r="AC4" s="19"/>
+      <c r="AD4" s="20"/>
+      <c r="AE4" s="11"/>
+    </row>
+    <row r="5" spans="1:31" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7">
+        <v>43768</v>
+      </c>
+      <c r="D5" s="9">
+        <v>43769</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="21"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="22"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="14"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="22"/>
+      <c r="AE5" s="26"/>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7">
+        <v>43770</v>
+      </c>
+      <c r="D6" s="9">
+        <v>43771</v>
+      </c>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="21"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="21"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="14"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="26"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="4"/>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="7">
+        <v>43772</v>
+      </c>
+      <c r="D7" s="9">
+        <v>43774</v>
+      </c>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="21"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="14"/>
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="21"/>
+      <c r="AB7" s="14"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="22"/>
+      <c r="AE7" s="26"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="7">
+        <v>43775</v>
+      </c>
+      <c r="D8" s="9">
+        <v>43777</v>
+      </c>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="14"/>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="21"/>
+      <c r="AB8" s="14"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="22"/>
+      <c r="AE8" s="26"/>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="8">
+        <v>43778</v>
+      </c>
+      <c r="D9" s="10"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="21"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="21"/>
+      <c r="AB9" s="14"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="22"/>
+      <c r="AE9" s="26"/>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="7">
+        <v>43779</v>
+      </c>
+      <c r="D10" s="9">
+        <v>43780</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="14"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="23"/>
+      <c r="U10" s="29"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="21"/>
+      <c r="AB10" s="14"/>
+      <c r="AC10" s="14"/>
+      <c r="AD10" s="22"/>
+      <c r="AE10" s="26"/>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="7">
+        <v>43781</v>
+      </c>
+      <c r="D11" s="9">
+        <v>43782</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="20"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="35"/>
+      <c r="W11" s="29"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="21"/>
+      <c r="AB11" s="14"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="22"/>
+      <c r="AE11" s="26"/>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="7">
+        <v>43783</v>
+      </c>
+      <c r="D12" s="9">
+        <v>43784</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="22"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="20"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="35"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="29"/>
+      <c r="AA12" s="21"/>
+      <c r="AB12" s="14"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="22"/>
+      <c r="AE12" s="26"/>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="7">
+        <v>43785</v>
+      </c>
+      <c r="D13" s="9">
+        <v>43787</v>
+      </c>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="20"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="23"/>
+      <c r="AB13" s="24"/>
+      <c r="AC13" s="24"/>
+      <c r="AD13" s="29"/>
+      <c r="AE13" s="26"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="7">
+        <v>43788</v>
+      </c>
+      <c r="D14" s="9">
+        <v>43791</v>
+      </c>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="14"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="21"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="21"/>
+      <c r="W14" s="22"/>
+      <c r="X14" s="28"/>
+      <c r="Y14" s="19"/>
+      <c r="Z14" s="20"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AC14" s="13"/>
+      <c r="AD14" s="13"/>
+      <c r="AE14" s="27"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="8">
+        <v>43792</v>
+      </c>
+      <c r="D15" s="10"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="24"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="27"/>
+      <c r="R15" s="23"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="29"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="29"/>
+      <c r="AA15" s="37"/>
+      <c r="AB15" s="32"/>
+      <c r="AC15" s="32"/>
+      <c r="AD15" s="31"/>
+      <c r="AE15" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="O2:S2"/>
-    <mergeCell ref="T2:X2"/>
-    <mergeCell ref="A3:B3"/>
+  <mergeCells count="21">
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="Z2:AE2"/>
+    <mergeCell ref="S2:Y2"/>
+    <mergeCell ref="L2:R2"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>